<commit_message>
make ui work part 1
</commit_message>
<xml_diff>
--- a/core/ColorInfo.xlsx
+++ b/core/ColorInfo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maddie/Documents/IW/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maddie/Documents/graphhopper/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Palmer Square East</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Hulfish Street</t>
+  </si>
+  <si>
+    <t>Nassau Street</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -100,6 +103,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -471,7 +475,12 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D9" s="2"/>
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D10" s="2"/>

</xml_diff>